<commit_message>
fix: remove password in xlxs upload student
</commit_message>
<xml_diff>
--- a/public/upload-student/ตัวอย่างข้อมูลนิสิตที่จะอัพโหลด.xlsx
+++ b/public/upload-student/ตัวอย่างข้อมูลนิสิตที่จะอัพโหลด.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stamp\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WORK\Bluelock007\Fronend-Bluelock-007\public\upload-student\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D357B73A-A361-4C85-A2FA-6D2594A58E68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30BDC960-96D6-4E5E-99BE-0FCAE142E498}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="37">
   <si>
     <t>name</t>
   </si>
@@ -496,10 +496,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z11"/>
+  <dimension ref="A1:Y11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" customHeight="1"/>
@@ -508,11 +508,10 @@
     <col min="2" max="2" width="32" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
     <col min="4" max="4" width="37" customWidth="1"/>
-    <col min="5" max="5" width="16.375" customWidth="1"/>
-    <col min="6" max="7" width="15" customWidth="1"/>
+    <col min="5" max="6" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="15.75">
+    <row r="1" spans="1:25" ht="15.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -526,14 +525,12 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="G1" s="2"/>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
@@ -552,9 +549,8 @@
       <c r="W1" s="2"/>
       <c r="X1" s="2"/>
       <c r="Y1" s="2"/>
-      <c r="Z1" s="2"/>
-    </row>
-    <row r="2" spans="1:26" ht="15" customHeight="1">
+    </row>
+    <row r="2" spans="1:25" ht="15" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>14</v>
       </c>
@@ -567,14 +563,14 @@
       <c r="D2" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="E2" s="2">
+        <v>31</v>
+      </c>
       <c r="F2" s="2">
-        <v>31</v>
-      </c>
-      <c r="G2" s="2">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="15" customHeight="1">
+    <row r="3" spans="1:25" ht="15" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
@@ -587,14 +583,14 @@
       <c r="D3" s="2" t="s">
         <v>25</v>
       </c>
+      <c r="E3" s="2">
+        <v>32</v>
+      </c>
       <c r="F3" s="2">
-        <v>32</v>
-      </c>
-      <c r="G3" s="2">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="15" customHeight="1">
+    <row r="4" spans="1:25" ht="15" customHeight="1">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
@@ -607,14 +603,14 @@
       <c r="D4" s="2" t="s">
         <v>26</v>
       </c>
+      <c r="E4" s="2">
+        <v>34</v>
+      </c>
       <c r="F4" s="2">
-        <v>34</v>
-      </c>
-      <c r="G4" s="2">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="15" customHeight="1">
+    <row r="5" spans="1:25" ht="15" customHeight="1">
       <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
@@ -627,14 +623,14 @@
       <c r="D5" s="2" t="s">
         <v>27</v>
       </c>
+      <c r="E5" s="2">
+        <v>33</v>
+      </c>
       <c r="F5" s="2">
-        <v>33</v>
-      </c>
-      <c r="G5" s="2">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="15" customHeight="1">
+    <row r="6" spans="1:25" ht="15" customHeight="1">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -647,14 +643,14 @@
       <c r="D6" s="2" t="s">
         <v>26</v>
       </c>
+      <c r="E6" s="2">
+        <v>38</v>
+      </c>
       <c r="F6" s="2">
-        <v>38</v>
-      </c>
-      <c r="G6" s="2">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="15.75" customHeight="1">
+    <row r="7" spans="1:25" ht="15.75" customHeight="1">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
@@ -667,12 +663,13 @@
       <c r="D7" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="E7" s="2">
+        <v>32</v>
+      </c>
       <c r="F7" s="2">
-        <v>32</v>
-      </c>
-      <c r="G7" s="2">
         <v>15</v>
       </c>
+      <c r="H7" s="2"/>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
@@ -690,9 +687,8 @@
       <c r="W7" s="2"/>
       <c r="X7" s="2"/>
       <c r="Y7" s="2"/>
-      <c r="Z7" s="2"/>
-    </row>
-    <row r="8" spans="1:26" ht="15.75" customHeight="1">
+    </row>
+    <row r="8" spans="1:25" ht="15.75" customHeight="1">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -705,12 +701,13 @@
       <c r="D8" s="2" t="s">
         <v>25</v>
       </c>
+      <c r="E8" s="2">
+        <v>36</v>
+      </c>
       <c r="F8" s="2">
-        <v>36</v>
-      </c>
-      <c r="G8" s="2">
         <v>19</v>
       </c>
+      <c r="H8" s="2"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
@@ -728,9 +725,9 @@
       <c r="W8" s="2"/>
       <c r="X8" s="2"/>
       <c r="Y8" s="2"/>
-      <c r="Z8" s="2"/>
-    </row>
-    <row r="9" spans="1:26" ht="15.75" customHeight="1">
+    </row>
+    <row r="9" spans="1:25" ht="15.75" customHeight="1">
+      <c r="H9" s="2"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
@@ -748,9 +745,9 @@
       <c r="W9" s="2"/>
       <c r="X9" s="2"/>
       <c r="Y9" s="2"/>
-      <c r="Z9" s="2"/>
-    </row>
-    <row r="10" spans="1:26" ht="15.75" customHeight="1">
+    </row>
+    <row r="10" spans="1:25" ht="15.75" customHeight="1">
+      <c r="H10" s="2"/>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
@@ -768,9 +765,9 @@
       <c r="W10" s="2"/>
       <c r="X10" s="2"/>
       <c r="Y10" s="2"/>
-      <c r="Z10" s="2"/>
-    </row>
-    <row r="11" spans="1:26" ht="15.75" customHeight="1">
+    </row>
+    <row r="11" spans="1:25" ht="15.75" customHeight="1">
+      <c r="H11" s="2"/>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
@@ -788,7 +785,6 @@
       <c r="W11" s="2"/>
       <c r="X11" s="2"/>
       <c r="Y11" s="2"/>
-      <c r="Z11" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>